<commit_message>
Avancement sur le MAN, manque développement
</commit_message>
<xml_diff>
--- a/Documentation/Devis Technique Prototype/!EvaluationCouts_malette&accessoire.xlsx
+++ b/Documentation/Devis Technique Prototype/!EvaluationCouts_malette&accessoire.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\cours\planif projet\Projet_Final_TSO\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Documentation\Devis Technique Prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C28847-5DD0-4999-8C92-EED8F1419DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B3224B-5A73-483E-8C83-1FFDDCA98803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste" sheetId="1" r:id="rId1"/>
     <sheet name="Infos" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -827,7 +827,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,9 +1170,10 @@
     <hyperlink ref="C7" r:id="rId2" xr:uid="{8FF5AA55-E3B9-449B-9CEE-03B53A6D7D4D}"/>
     <hyperlink ref="C8" r:id="rId3" xr:uid="{C3DB5301-BBB3-4D06-B4C1-3C86DB8B7CA1}"/>
     <hyperlink ref="C9" r:id="rId4" xr:uid="{4ED08511-B353-4D99-9D89-C9C44BE27896}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{922C5FD8-CC5F-43D0-B594-C268F057C323}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="76" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId5"/>
+  <pageSetup scale="76" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1232,6 +1233,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DDF7F2FCC1D2C469E7882E767051E21" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fdb502a7565e043baea1e7044cb52160">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de9a939f-7971-4532-9b84-38cbdf21fdbe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87cf97e6ee09886aa213502e86bb7644" ns2:_="">
     <xsd:import namespace="de9a939f-7971-4532-9b84-38cbdf21fdbe"/>
@@ -1375,22 +1391,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{933EE957-C7CB-4D6D-82A9-7153ECCB8F4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="59f032a8-2326-4110-a897-48ad6ab7eae4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{680BFF76-E453-4BF1-ABDD-4FE67DE99218}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1406,22 +1425,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E95A2D-E86D-4BB2-B369-D2BBA7B4865E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{933EE957-C7CB-4D6D-82A9-7153ECCB8F4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="59f032a8-2326-4110-a897-48ad6ab7eae4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>